<commit_message>
updated user guide, sample data, fix issue
</commit_message>
<xml_diff>
--- a/testdata/danhsachcongdoan.xlsx
+++ b/testdata/danhsachcongdoan.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Anh\MTGNT\hrm_monastery\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/worker/work/github/hrm_monastery/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C1FFA2-5D54-2340-BFEC-B2A5D4E19057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comm" sheetId="1" r:id="rId1"/>
-    <sheet name="MA_QUOC_GIA" sheetId="2" r:id="rId2"/>
+    <sheet name="TRANG_THAI" sheetId="3" r:id="rId2"/>
+    <sheet name="MA_QUOC_GIA" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="428">
   <si>
     <t>#</t>
   </si>
@@ -1241,21 +1243,6 @@
   </si>
   <si>
     <t>Zimbabwe</t>
-  </si>
-  <si>
-    <t>Cộng đoàn Thủ Đức</t>
-  </si>
-  <si>
-    <t>Cộng Đoàn Mỹ</t>
-  </si>
-  <si>
-    <t>Hoa kỳ</t>
-  </si>
-  <si>
-    <t>31/1</t>
-  </si>
-  <si>
-    <t>31/12/2023</t>
   </si>
   <si>
     <t>địa chỉ</t>
@@ -1278,16 +1265,61 @@
   <si>
     <t>Ngày bổn mạng
 Ngày/Tháng</t>
+  </si>
+  <si>
+    <t>Cộng đoàn Mến Thánh Giá Thủ Thiêm</t>
+  </si>
+  <si>
+    <t>Cộng đoàn Mến Thánh Giá Phan Thiết</t>
+  </si>
+  <si>
+    <t>20/12</t>
+  </si>
+  <si>
+    <t>4/5</t>
+  </si>
+  <si>
+    <t>20/10/2022</t>
+  </si>
+  <si>
+    <t>1/10/2000</t>
+  </si>
+  <si>
+    <t>congdoan@gmail.com</t>
+  </si>
+  <si>
+    <t>Mã Trạng Thái</t>
+  </si>
+  <si>
+    <t>Trạng Thái</t>
+  </si>
+  <si>
+    <t>Không rõ</t>
+  </si>
+  <si>
+    <t>Không hoạt động</t>
+  </si>
+  <si>
+    <t>Đang hoạt động</t>
+  </si>
+  <si>
+    <t>Đang xây dựng</t>
+  </si>
+  <si>
+    <t>Chưa sẵng sàng</t>
+  </si>
+  <si>
+    <t>MA_TINH_TRANG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -1299,6 +1331,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1320,21 +1359,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1350,10 +1392,208 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC134C6C-20EA-3DAC-7D16-26200A7A385A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3695700" y="406400"/>
+          <a:ext cx="6515100" cy="927100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Thông tin trạng thái có thể nhập</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Đây là thông tin tham khảo</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Cần đồng bộ với dữ liệu trên ứng dụng</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86E2F3AC-DE13-6E4F-832B-85C774118B25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4305300" y="584200"/>
+          <a:ext cx="6515100" cy="927100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Thông tin Quốc Gia</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Đây là thông tin tham khảo</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Cần đồng bộ với dữ liệu trên ứng dụng</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1391,9 +1631,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1428,7 +1668,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1463,7 +1703,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1636,51 +1876,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.875" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.125" customWidth="1"/>
-    <col min="10" max="10" width="15.375" customWidth="1"/>
-    <col min="11" max="11" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.875" customWidth="1"/>
-    <col min="13" max="13" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.1640625" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.83203125" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D1" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>416</v>
-      </c>
-      <c r="F1" s="1" t="s">
+    <row r="1" spans="1:14" ht="34">
+      <c r="D1" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1691,1676 +1935,1757 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="E3" s="4">
-        <v>36526</v>
-      </c>
-      <c r="F3" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1"/>
-      <c r="L3" s="1" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="M3" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="D4" s="3">
-        <v>45269</v>
+        <v>414</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="1"/>
-      <c r="L4" t="s">
+        <v>416</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="I4" s="1">
+        <v>903365456</v>
+      </c>
+      <c r="M4" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H4" r:id="rId1" xr:uid="{88A42AAC-DE57-4B41-8F2F-AEF8DE81F9D7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B198"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104760BD-4F62-824F-84C8-103EF30AB37F}">
+  <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="A195" sqref="A195"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B196"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B51" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B52" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B53" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B56" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B57" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B58" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B59" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B60" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B61" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B62" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B63" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B64" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B65" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B66" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B67" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B68" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B69" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B70" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B71" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B72" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B73" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B74" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B75" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B76" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B77" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B78" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B79" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B80" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B81" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B82" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B83" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B84" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B85" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B86" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B87" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B88" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B89" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B90" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B91" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B92" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B93" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B94" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B95" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B96" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B97" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B98" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B99" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B100" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B101" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B102" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B103" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B104" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B105" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B106" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B107" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B108" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B109" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B110" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B111" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B112" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B113" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B114" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B115" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B116" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B117" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B118" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B119" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B120" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B121" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B122" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B123" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B124" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B125" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B126" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B127" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B128" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B129" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B130" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B131" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B132" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B133" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B134" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B135" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B136" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="B137" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B138" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B139" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B140" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B141" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B142" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B143" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B144" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B145" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B146" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B147" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B148" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B149" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="B150" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B151" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B152" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B153" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B154" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B155" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B156" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B157" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B158" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B159" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B160" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B161" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="B162" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B163" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B164" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B165" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="B166" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="B167" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="B168" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="B169" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B170" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B171" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B172" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B173" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B174" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="B175" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B176" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="B177" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="B178" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B179" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B180" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="B181" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="B182" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B183" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B184" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="B185" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="B186" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B187" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>385</v>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" s="1" t="s">
+        <v>389</v>
       </c>
       <c r="B188" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="B189" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="1" t="s">
-        <v>389</v>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
+        <v>393</v>
       </c>
       <c r="B190" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B191" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="B192" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B193" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="B194" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B195" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="B196" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>403</v>
-      </c>
-      <c r="B197" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>405</v>
-      </c>
-      <c r="B198" t="s">
         <v>406</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>